<commit_message>
[IMP] tables: export table style in xlsx
Task: 3789612
Part-of: odoo/o-spreadsheet#3799
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\odoo\spreadsheet\tests\__xlsx__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676AF7E1-BB07-416E-B55F-CE934DA012B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C606C4-F84F-45BF-8292-2BBF6330484B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="21705" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2211,217 +2211,6 @@
   </cellStyles>
   <dxfs count="44">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike/>
-        <u/>
-        <color theme="7"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="lightTrellis">
-          <fgColor theme="4"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2693,25 +2482,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -2761,6 +2531,236 @@
       <fill>
         <patternFill>
           <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike/>
+        <u/>
+        <color theme="7"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="lightTrellis">
+          <fgColor theme="4"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4807,6 +4807,741 @@
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2200"/>
+              <a:t>scatter chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1000-4695-A558-70E3A3698455}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="17781237"/>
+        <c:axId val="88853993"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="17781237"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="1"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1000" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88853993"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="88853993"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="1"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1000" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17781237"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr sz="1000" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln cmpd="sng">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2200"/>
+              <a:t>combo chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="1F77B4"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="1F77B4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Emily Anderson (Emmy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sophie Allen (Saffi)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chloe Adams</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Megan Alexander (Meg)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lucy Arnold (Lulu)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hannah Alvarez</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jessica Alcock (Jess)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Charlotte Anaya</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lauren Anthony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:srgbClr val="1F77B4"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-457C-469E-B304-7A21AF960744}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="70"/>
+        <c:axId val="17781237"/>
+        <c:axId val="88853993"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF7F0E"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Emily Anderson (Emmy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sophie Allen (Saffi)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chloe Adams</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Megan Alexander (Meg)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lucy Arnold (Lulu)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hannah Alvarez</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jessica Alcock (Jess)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Charlotte Anaya</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lauren Anthony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-457C-469E-B304-7A21AF960744}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="17781237"/>
+        <c:axId val="88853993"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="17781237"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="1"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1000" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88853993"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88853993"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="1"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1000" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17781237"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr sz="1000" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln cmpd="sng">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
+  <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
@@ -4926,7 +5661,7 @@
               </c14:invertSolidFillFmt>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DE95-4F98-865F-6E35D6C9378D}"/>
+              <c16:uniqueId val="{00000000-D94B-45A0-8AD6-3E4F4E7665C2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5042,7 +5777,7 @@
               </c14:invertSolidFillFmt>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DE95-4F98-865F-6E35D6C9378D}"/>
+              <c16:uniqueId val="{00000001-D94B-45A0-8AD6-3E4F4E7665C2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5838,6 +6573,82 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 4" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CC27214-40A9-4FF9-BB37-40F876B2768B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 6" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5685A00-859E-4641-A529-E7042819F3BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6247,7 +7058,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -6259,22 +7070,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6669,7 +7480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3FFA98-6851-421C-959C-388F2B66EDF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385D5EBC-45F5-4C42-AA75-560DF70B9F2E}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
@@ -7076,7 +7887,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7119,7 +7930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B780FB99-17EE-4EC6-9495-0F952AB94F6F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7A934C-2218-4A12-8B75-EE28D615D774}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -7133,15 +7944,15 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43501D2F-A9B0-48FF-8DF0-12CB4DAF54E6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96301BE1-D86D-4D45-870D-85A75D53FC99}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="G23" sqref="G23"/>
-      <selection pane="topRight" activeCell="G23" sqref="G23"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
-      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
+      <selection activeCell="H9" sqref="H9"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7151,7 +7962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FD2198-2564-4D41-B915-30691D7E40F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10A8834-0E20-4F80-8813-3ACA5527B377}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7170,7 +7981,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FD2250-DC4A-49ED-86BD-0294A74D37AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{410DDE30-90F0-4479-AC28-0576838C0CFE}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -7186,7 +7997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADB4250-469A-495C-8211-7D36C3F1DFC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0630FA18-71FC-4ACD-8379-39A3603D1DD6}">
   <dimension ref="A1:R163"/>
   <sheetViews>
     <sheetView topLeftCell="A97" workbookViewId="0">
@@ -9046,7 +9857,7 @@
       </c>
       <c r="B100" s="20">
         <f ca="1">NOW()</f>
-        <v>45359.413205787037</v>
+        <v>45398.575743402776</v>
       </c>
       <c r="D100" s="2">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
@@ -9736,7 +10547,7 @@
       </c>
       <c r="B144" s="19">
         <f ca="1">TODAY()</f>
-        <v>45359</v>
+        <v>45398</v>
       </c>
       <c r="D144" s="2">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
@@ -10050,10 +10861,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10062,7 +10873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B9D0FD-8DC8-4D93-B94A-6AB101FCCDA5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FE33AE-060F-4630-8DDE-76E5F5CF58F5}">
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
@@ -10153,11 +10964,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C120773E-1A0C-4228-98C5-817652C8CC14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF68F2C0-1053-4FB6-BD74-8A11B0CAF123}">
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10544,7 +11355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF5F2C6-E886-4E2A-B7A1-398EDD6A725D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D919E811-4385-4D35-A19E-3B7E0E659A89}">
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -10780,7 +11591,7 @@
       </c>
       <c r="B12" s="40">
         <f ca="1">TODAY()</f>
-        <v>45359</v>
+        <v>45398</v>
       </c>
       <c r="C12" s="40">
         <f>DATE(2010,10,2)</f>
@@ -11313,70 +12124,142 @@
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="expression" dxfId="22" priority="58">
+      <formula>ODD(B15)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:B27">
+    <cfRule type="cellIs" dxfId="21" priority="46" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C2">
+    <cfRule type="aboveAverage" dxfId="20" priority="114"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="43" priority="73" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="19" priority="73" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="42" priority="71">
+    <cfRule type="containsBlanks" dxfId="18" priority="71">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="41" priority="70">
+    <cfRule type="containsErrors" dxfId="17" priority="70">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="40" priority="69" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="16" priority="69" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="39" priority="67" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="15" priority="67" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="66">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="37" priority="65">
+    <cfRule type="notContainsErrors" dxfId="13" priority="65">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="36" priority="64" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="12" priority="64" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="35" priority="63" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="11" priority="63" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="34" priority="58">
-      <formula>ODD(B15)</formula>
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="top10" dxfId="10" priority="115" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:C16">
+    <cfRule type="cellIs" dxfId="9" priority="45" operator="equal">
+      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="33" priority="56" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="56" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="32" priority="46" operator="equal">
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="31" priority="45" operator="equal">
+  <conditionalFormatting sqref="B19:C19">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:C20">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:C21">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:C22">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+      <formula>2</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:C23">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="notBetween">
+      <formula>2</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:C24">
+    <cfRule type="dataBar" priority="100">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{88E4E898-A83E-4EE8-B4ED-3339A906DC10}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:C25">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C2002CEC-3733-4955-A6B6-FF982F2050DC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:D7">
+    <cfRule type="duplicateValues" dxfId="1" priority="82"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:D14">
+    <cfRule type="uniqueValues" dxfId="0" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="44">
@@ -11539,32 +12422,6 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="30" priority="82"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="29" priority="96"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:C24">
-    <cfRule type="dataBar" priority="100">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63C384"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{88E4E898-A83E-4EE8-B4ED-3339A906DC10}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="28" priority="114"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="27" priority="115" rank="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H21:K21">
     <cfRule type="iconSet" priority="18">
       <iconSet iconSet="4Arrows">
@@ -11659,52 +12516,6 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="greaterThan">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThan">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="lessThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="between">
-      <formula>2</formula>
-      <formula>4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="notBetween">
-      <formula>2</formula>
-      <formula>4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B25:C25">
-    <cfRule type="dataBar" priority="7">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63C384"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C2002CEC-3733-4955-A6B6-FF982F2050DC}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
@@ -11731,6 +12542,57 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>B25:C25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="20" id="{0776DCAB-3210-41C4-A113-32FD4847A5ED}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H19:J19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="19" id="{367C8C3A-A19C-489B-B02C-135E717D92A5}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H20:J20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="8" id="{2F0448E0-FD4B-4CC6-8AFB-1FCD78ED3F40}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H31:J31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="25" id="{EDB615C5-C26E-42E3-8D7C-CFC96E348794}">
@@ -11790,38 +12652,6 @@
           <xm:sqref>H37:J37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="20" id="{0776DCAB-3210-41C4-A113-32FD4847A5ED}">
-            <x14:iconSet iconSet="3Stars">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>33</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>67</xm:f>
-              </x14:cfvo>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>H19:J19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="19" id="{367C8C3A-A19C-489B-B02C-135E717D92A5}">
-            <x14:iconSet iconSet="3Triangles">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>33</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>67</xm:f>
-              </x14:cfvo>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>H20:J20</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="9" id="{DD78C548-721C-42F8-BA23-99215A699C4C}">
             <x14:iconSet iconSet="5Boxes">
               <x14:cfvo type="percent">
@@ -11843,25 +12673,6 @@
           </x14:cfRule>
           <xm:sqref>H30:L30</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{2F0448E0-FD4B-4CC6-8AFB-1FCD78ED3F40}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>33</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>67</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>H31:J31</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -11869,10 +12680,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA2AD09-EFB1-4B74-862F-432090DD90CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CCC4B1-5C65-4837-AA26-56CCF06B63BB}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12198,7 +13011,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E49991F-68D4-4649-AFDB-79BBFCE497F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9224F2-4D06-4586-886C-E51F5EBCA7B0}">
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12515,7 +13328,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1BCB21-6252-4834-AE7A-48E70B5AD55E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -12556,7 +13369,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B93B36-2628-4853-9774-0EB7977881CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE31E21-0350-44E7-AF13-4CA140505B30}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>

<commit_message>
[IMP] tables: import table styles in xlsx
This commit adds the conversion of table style from xlsx to
o-spreadsheet.

The xlsx pivots are now handled separately fro the tables, as they have
a slightly different configuration.

Task: 3789612
Part-of: odoo/o-spreadsheet#3799
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C606C4-F84F-45BF-8292-2BBF6330484B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0F1A66-FDA3-41D2-8301-AC5DB36FDC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2430" windowWidth="21705" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="417">
   <si>
     <t>CF =42</t>
   </si>
@@ -1298,12 +1298,15 @@
   </si>
   <si>
     <t>'sheet!'!R[1]C[1]</t>
+  </si>
+  <si>
+    <t>CustomStyle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ hh:mm:ss"/>
@@ -2209,7 +2212,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="46">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2765,7 +2782,12 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{33B8EB55-D8D8-4B00-B5CF-C84A8AC9E775}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="firstRowStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FF000000"/>
@@ -7058,7 +7080,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -7070,26 +7092,36 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="1" showLastColumn="1" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A957E632-0695-4531-8323-5048B676464D}" name="Table2" displayName="Table2" ref="C34:D35" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{DC5A2AE6-F19E-430A-B1C3-28F7319B94EE}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{2050F373-1538-4D53-8D8B-FBE687F1DDF5}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -7887,7 +7919,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7947,7 +7979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96301BE1-D86D-4D45-870D-85A75D53FC99}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H9" sqref="H9"/>
       <selection pane="topRight" activeCell="H9" sqref="H9"/>
@@ -9857,7 +9889,7 @@
       </c>
       <c r="B100" s="20">
         <f ca="1">NOW()</f>
-        <v>45398.575743402776</v>
+        <v>45398.580923148147</v>
       </c>
       <c r="D100" s="2">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
@@ -10861,10 +10893,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10967,7 +10999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF68F2C0-1053-4FB6-BD74-8A11B0CAF123}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -12125,104 +12157,104 @@
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="22" priority="58">
+    <cfRule type="expression" dxfId="24" priority="58">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="21" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="20" priority="114"/>
+    <cfRule type="aboveAverage" dxfId="22" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="19" priority="73" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="21" priority="73" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="18" priority="71">
+    <cfRule type="containsBlanks" dxfId="20" priority="71">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="17" priority="70">
+    <cfRule type="containsErrors" dxfId="19" priority="70">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="16" priority="69" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="18" priority="69" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="15" priority="67" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="17" priority="67" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="66">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="13" priority="65">
+    <cfRule type="notContainsErrors" dxfId="15" priority="65">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="12" priority="64" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="14" priority="64" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="11" priority="63" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="13" priority="63" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="10" priority="115" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="115" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="9" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="45" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="8" priority="56" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="56" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
@@ -12256,10 +12288,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="1" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="0" priority="96"/>
+    <cfRule type="uniqueValues" dxfId="2" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="44">
@@ -12681,10 +12713,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CCC4B1-5C65-4837-AA26-56CCF06B63BB}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12994,9 +13026,14 @@
         <v>408</v>
       </c>
     </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>416</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="9">
+  <tableParts count="10">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -13006,6 +13043,7 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
@@ -13331,7 +13369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[IMP] charts: add radar chart
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\odoo\spreadsheet\tests\__xlsx__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05E556DF-B6A9-4914-8E28-82201545992C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EAB923-A1B3-42FF-B544-1E3FCDFFEEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,9 @@
   <externalReferences>
     <externalReference r:id="rId14"/>
   </externalReferences>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="153" r:id="rId15"/>
+    <pivotCache cacheId="0" r:id="rId15"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,8 +45,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1321,7 +1319,7 @@
     <numFmt numFmtId="169" formatCode="#,##0&quot; EUR €&quot;"/>
     <numFmt numFmtId="170" formatCode="&quot;€&quot;#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2198,6 +2196,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2210,165 +2209,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
   <dxfs count="46">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike/>
-        <u/>
-        <color theme="7"/>
-      </font>
-      <numFmt numFmtId="171" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="lightTrellis">
-          <fgColor theme="4"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2775,6 +2622,157 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike/>
+        <u/>
+        <color theme="7"/>
+      </font>
+      <numFmt numFmtId="171" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="lightTrellis">
+          <fgColor theme="4"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
@@ -2818,7 +2816,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2874,7 +2872,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3196,7 +3194,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3229,7 +3227,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="88853993"/>
@@ -3300,7 +3298,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3333,7 +3331,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="17781237"/>
@@ -3377,7 +3375,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3405,7 +3403,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3419,7 +3417,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -3732,7 +3730,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="88853993"/>
@@ -3794,7 +3792,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="17781237"/>
@@ -3822,7 +3820,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3851,7 +3849,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -4440,7 +4438,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4469,7 +4467,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4806,7 +4804,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4835,7 +4833,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -5018,7 +5016,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="88853993"/>
@@ -5077,7 +5075,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="17781237"/>
@@ -5105,7 +5103,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5134,7 +5132,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5451,7 +5449,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="88853993"/>
@@ -5513,7 +5511,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="17781237"/>
@@ -5541,7 +5539,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5570,7 +5568,412 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2200"/>
+              <a:t>radar chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="1F77B4"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="1F77B4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Emily Anderson (Emmy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sophie Allen (Saffi)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chloe Adams</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Megan Alexander (Meg)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lucy Arnold (Lulu)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hannah Alvarez</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jessica Alcock (Jess)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Charlotte Anaya</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lauren Anthony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E3B9-4952-B105-568BDB7EC1F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF7F0E"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Emily Anderson (Emmy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sophie Allen (Saffi)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chloe Adams</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Megan Alexander (Meg)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lucy Arnold (Lulu)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hannah Alvarez</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jessica Alcock (Jess)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Charlotte Anaya</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lauren Anthony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E3B9-4952-B105-568BDB7EC1F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="17781237"/>
+        <c:axId val="88853993"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="17781237"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="1"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1000" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88853993"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88853993"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="1"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1000" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17781237"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr sz="1000" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln cmpd="sng">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -5868,7 +6271,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="344680958"/>
@@ -5944,7 +6347,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="998664793"/>
@@ -5967,7 +6370,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6684,6 +7087,44 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>70485</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 6" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B20B98-FA84-44C9-8DBB-5852658E9967}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6943,7 +7384,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="153" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -7093,7 +7534,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -7105,22 +7546,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="9">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="7">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7230,7 +7671,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7531,20 +7972,20 @@
   </sheetPr>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="26" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="26" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -7553,7 +7994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="27.75">
+    <row r="2" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="B2" s="23" t="s">
         <v>2</v>
       </c>
@@ -7566,25 +8007,25 @@
       <c r="H2" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="110"/>
+      <c r="I2" s="106"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2">
         <v>8</v>
       </c>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="106">
+      <c r="K3" s="107">
         <v>5</v>
       </c>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
@@ -7597,50 +8038,50 @@
       <c r="G4" s="2">
         <v>9</v>
       </c>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="107"/>
+      <c r="K4" s="108"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2">
         <v>42</v>
       </c>
       <c r="G5" s="2">
         <v>15</v>
       </c>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="107"/>
+      <c r="K5" s="108"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G6" s="2">
         <v>22</v>
       </c>
       <c r="J6" s="6"/>
-      <c r="K6" s="107"/>
+      <c r="K6" s="108"/>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2">
         <v>3</v>
       </c>
       <c r="J7" s="6"/>
-      <c r="K7" s="107"/>
+      <c r="K7" s="108"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G8" s="2">
         <v>30</v>
       </c>
       <c r="J8" s="6"/>
-      <c r="K8" s="108"/>
+      <c r="K8" s="109"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" ht="17.25" customHeight="1">
+    <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
@@ -7650,7 +8091,7 @@
       </c>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2">
         <f>SUM(C4:C7)</f>
         <v>57.4</v>
@@ -7659,13 +8100,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.25" customHeight="1">
+    <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2">
         <f>-(3+C7*SUM(C4:C7))</f>
         <v>-175.2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.25" customHeight="1">
+    <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2">
         <f>SUM(C9:C11)</f>
         <v>-63.399999999999991</v>
@@ -7674,13 +8115,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.25" customHeight="1">
+    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G13" s="2">
         <f>A1+A2+A3+A4+A5+A6+A7+A8+A9+A10+A11+A12+A13+A14+A15+A16+A17+A18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.25" customHeight="1">
+    <row r="14" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
         <v>11</v>
       </c>
@@ -7689,32 +8130,32 @@
         <v>#CYCLE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.25" customHeight="1">
+    <row r="15" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17.25" customHeight="1">
+    <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="str">
         <f>C15</f>
         <v>=(+</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17.25" customHeight="1">
+    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.25" customHeight="1">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17.25" customHeight="1">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
         <v>15</v>
@@ -7728,7 +8169,7 @@
       </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" customHeight="1">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>18</v>
       </c>
@@ -7738,7 +8179,7 @@
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>19</v>
       </c>
@@ -7752,7 +8193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="17">
         <v>10</v>
       </c>
@@ -7763,7 +8204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="17">
         <v>10.122999999999999</v>
       </c>
@@ -7774,7 +8215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
@@ -7788,7 +8229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -7805,7 +8246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>23</v>
       </c>
@@ -7822,7 +8263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
@@ -7839,7 +8280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
@@ -7856,7 +8297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
@@ -7873,7 +8314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>27</v>
       </c>
@@ -7890,7 +8331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="17.25" customHeight="1">
+    <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
@@ -7907,7 +8348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="17.25" customHeight="1">
+    <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
@@ -7918,7 +8359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17.25" customHeight="1">
+    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
@@ -7935,7 +8376,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7985,7 +8426,7 @@
       <selection sqref="A1:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7997,12 +8438,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
       <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8016,10 +8457,10 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="26" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="65.109375" customWidth="1"/>
+    <col min="2" max="26" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8036,7 +8477,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8054,12 +8495,12 @@
       <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="26" width="13.7109375" customWidth="1"/>
+    <col min="1" max="26" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.25" customHeight="1">
+    <row r="1" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -8094,7 +8535,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1">
+    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
@@ -8140,7 +8581,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -8186,7 +8627,7 @@
         <v>1217.7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17.25" customHeight="1">
+    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -8232,7 +8673,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.25" customHeight="1">
+    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -8278,7 +8719,7 @@
         <v>1246.7</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17.25" customHeight="1">
+    <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -8324,7 +8765,7 @@
         <v>1213.7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17.25" customHeight="1">
+    <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -8358,7 +8799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17.25" customHeight="1">
+    <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -8392,7 +8833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17.25" customHeight="1">
+    <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
@@ -8423,7 +8864,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17.25" customHeight="1">
+    <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
@@ -8439,7 +8880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="17.25" customHeight="1">
+    <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
@@ -8458,7 +8899,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="17.25" customHeight="1">
+    <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>61</v>
       </c>
@@ -8489,7 +8930,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="17.25" customHeight="1">
+    <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
@@ -8520,7 +8961,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="17.25" customHeight="1">
+    <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>67</v>
       </c>
@@ -8536,7 +8977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="17.25" customHeight="1">
+    <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>68</v>
       </c>
@@ -8552,7 +8993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17.25" customHeight="1">
+    <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>69</v>
       </c>
@@ -8568,7 +9009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
@@ -8584,7 +9025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1">
+    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>71</v>
       </c>
@@ -8600,7 +9041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1">
+    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>72</v>
       </c>
@@ -8616,7 +9057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1">
+    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>73</v>
       </c>
@@ -8632,7 +9073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1">
+    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>74</v>
       </c>
@@ -8648,7 +9089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1">
+    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>76</v>
       </c>
@@ -8664,7 +9105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1">
+    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>77</v>
       </c>
@@ -8680,7 +9121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.25" customHeight="1">
+    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>78</v>
       </c>
@@ -8697,7 +9138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.25" customHeight="1">
+    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>79</v>
       </c>
@@ -8713,7 +9154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.25" customHeight="1">
+    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>81</v>
       </c>
@@ -8729,7 +9170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.25" customHeight="1">
+    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>82</v>
       </c>
@@ -8745,7 +9186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.25" customHeight="1">
+    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>83</v>
       </c>
@@ -8762,7 +9203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.25" customHeight="1">
+    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>84</v>
       </c>
@@ -8778,7 +9219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.25" customHeight="1">
+    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>85</v>
       </c>
@@ -8794,7 +9235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" customHeight="1">
+    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>86</v>
       </c>
@@ -8810,7 +9251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.25" customHeight="1">
+    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>87</v>
       </c>
@@ -8826,7 +9267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.25" customHeight="1">
+    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>88</v>
       </c>
@@ -8842,7 +9283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17.25" customHeight="1">
+    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>89</v>
       </c>
@@ -8858,7 +9299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.25" customHeight="1">
+    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>90</v>
       </c>
@@ -8874,7 +9315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.25" customHeight="1">
+    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>91</v>
       </c>
@@ -8890,7 +9331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.25" customHeight="1">
+    <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>92</v>
       </c>
@@ -8906,7 +9347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17.25" customHeight="1">
+    <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>93</v>
       </c>
@@ -8923,7 +9364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17.25" customHeight="1">
+    <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>94</v>
       </c>
@@ -8939,7 +9380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17.25" customHeight="1">
+    <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>95</v>
       </c>
@@ -8955,7 +9396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17.25" customHeight="1">
+    <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>96</v>
       </c>
@@ -8971,7 +9412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.25" customHeight="1">
+    <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>97</v>
       </c>
@@ -8987,7 +9428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17.25" customHeight="1">
+    <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>98</v>
       </c>
@@ -9003,7 +9444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.25" customHeight="1">
+    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>99</v>
       </c>
@@ -9019,7 +9460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.25" customHeight="1">
+    <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>100</v>
       </c>
@@ -9035,7 +9476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.25" customHeight="1">
+    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>101</v>
       </c>
@@ -9051,7 +9492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.25" customHeight="1">
+    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>102</v>
       </c>
@@ -9067,7 +9508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25" customHeight="1">
+    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>103</v>
       </c>
@@ -9083,7 +9524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17.25" customHeight="1">
+    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
@@ -9099,7 +9540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1">
+    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>105</v>
       </c>
@@ -9116,7 +9557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1">
+    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>106</v>
       </c>
@@ -9133,7 +9574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1">
+    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>107</v>
       </c>
@@ -9149,7 +9590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1">
+    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>108</v>
       </c>
@@ -9165,7 +9606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1">
+    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>109</v>
       </c>
@@ -9181,7 +9622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1">
+    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>110</v>
       </c>
@@ -9197,7 +9638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1">
+    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>111</v>
       </c>
@@ -9213,7 +9654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1">
+    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
@@ -9229,7 +9670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1">
+    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>113</v>
       </c>
@@ -9245,7 +9686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1">
+    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>114</v>
       </c>
@@ -9261,7 +9702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1">
+    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>115</v>
       </c>
@@ -9277,7 +9718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1">
+    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>116</v>
       </c>
@@ -9293,7 +9734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1">
+    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>117</v>
       </c>
@@ -9309,7 +9750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1">
+    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>118</v>
       </c>
@@ -9325,7 +9766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1">
+    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>119</v>
       </c>
@@ -9341,7 +9782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1">
+    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>120</v>
       </c>
@@ -9357,7 +9798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1">
+    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>121</v>
       </c>
@@ -9373,7 +9814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1">
+    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>122</v>
       </c>
@@ -9389,7 +9830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1">
+    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>123</v>
       </c>
@@ -9405,7 +9846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1">
+    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>125</v>
       </c>
@@ -9421,7 +9862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1">
+    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>127</v>
       </c>
@@ -9437,7 +9878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1">
+    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>129</v>
       </c>
@@ -9453,7 +9894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1">
+    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>130</v>
       </c>
@@ -9469,7 +9910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1">
+    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>131</v>
       </c>
@@ -9485,7 +9926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1">
+    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>132</v>
       </c>
@@ -9501,7 +9942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1">
+    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>133</v>
       </c>
@@ -9517,7 +9958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1">
+    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>134</v>
       </c>
@@ -9533,7 +9974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1">
+    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>135</v>
       </c>
@@ -9549,7 +9990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1">
+    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>136</v>
       </c>
@@ -9565,7 +10006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1">
+    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>137</v>
       </c>
@@ -9581,7 +10022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1">
+    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>138</v>
       </c>
@@ -9597,7 +10038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1">
+    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>139</v>
       </c>
@@ -9613,7 +10054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1">
+    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>141</v>
       </c>
@@ -9629,7 +10070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="17.25" customHeight="1">
+    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>142</v>
       </c>
@@ -9645,7 +10086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="17.25" customHeight="1">
+    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>143</v>
       </c>
@@ -9661,7 +10102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="17.25" customHeight="1">
+    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>144</v>
       </c>
@@ -9677,7 +10118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1">
+    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>146</v>
       </c>
@@ -9693,7 +10134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="17.25" customHeight="1">
+    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>147</v>
       </c>
@@ -9709,7 +10150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="17.25" customHeight="1">
+    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>148</v>
       </c>
@@ -9725,7 +10166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1">
+    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>149</v>
       </c>
@@ -9741,7 +10182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="17.25" customHeight="1">
+    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>150</v>
       </c>
@@ -9757,7 +10198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1">
+    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>151</v>
       </c>
@@ -9773,7 +10214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="17.25" customHeight="1">
+    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>152</v>
       </c>
@@ -9789,7 +10230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="17.25" customHeight="1">
+    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>153</v>
       </c>
@@ -9805,7 +10246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="17.25" customHeight="1">
+    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>154</v>
       </c>
@@ -9821,7 +10262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="17.25" customHeight="1">
+    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>155</v>
       </c>
@@ -9837,7 +10278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="17.25" customHeight="1">
+    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>156</v>
       </c>
@@ -9853,7 +10294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="17.25" customHeight="1">
+    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>157</v>
       </c>
@@ -9869,7 +10310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="17.25" customHeight="1">
+    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>158</v>
       </c>
@@ -9885,7 +10326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="17.25" customHeight="1">
+    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>159</v>
       </c>
@@ -9901,20 +10342,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="17.25" customHeight="1">
+    <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B100" s="20">
         <f ca="1">NOW()</f>
-        <v>45526.511599421297</v>
+        <v>45538.429115162035</v>
       </c>
       <c r="D100" s="2">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="17.25" customHeight="1">
+    <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>161</v>
       </c>
@@ -9930,7 +10371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="17.25" customHeight="1">
+    <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>162</v>
       </c>
@@ -9946,7 +10387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="17.25" customHeight="1">
+    <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>163</v>
       </c>
@@ -9962,7 +10403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="17.25" customHeight="1">
+    <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>164</v>
       </c>
@@ -9978,7 +10419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17.25" customHeight="1">
+    <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>165</v>
       </c>
@@ -9994,7 +10435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17.25" customHeight="1">
+    <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>166</v>
       </c>
@@ -10010,7 +10451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17.25" customHeight="1">
+    <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>167</v>
       </c>
@@ -10026,7 +10467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="17.25" customHeight="1">
+    <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>168</v>
       </c>
@@ -10042,7 +10483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="17.25" customHeight="1">
+    <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>169</v>
       </c>
@@ -10058,7 +10499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="17.25" customHeight="1">
+    <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>170</v>
       </c>
@@ -10074,7 +10515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="17.25" customHeight="1">
+    <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>171</v>
       </c>
@@ -10090,12 +10531,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="17.25" customHeight="1">
+    <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:4" ht="17.25" customHeight="1">
+    <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>172</v>
       </c>
@@ -10111,7 +10552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="17.25" customHeight="1">
+    <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>173</v>
       </c>
@@ -10127,7 +10568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="17.25" customHeight="1">
+    <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>175</v>
       </c>
@@ -10143,7 +10584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="17.25" customHeight="1">
+    <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>177</v>
       </c>
@@ -10159,7 +10600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="17.25" customHeight="1">
+    <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>178</v>
       </c>
@@ -10175,7 +10616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="17.25" customHeight="1">
+    <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>179</v>
       </c>
@@ -10191,7 +10632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="17.25" customHeight="1">
+    <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>180</v>
       </c>
@@ -10207,7 +10648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="17.25" customHeight="1">
+    <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>181</v>
       </c>
@@ -10223,7 +10664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="17.25" customHeight="1">
+    <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>182</v>
       </c>
@@ -10239,7 +10680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="17.25" customHeight="1">
+    <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>183</v>
       </c>
@@ -10255,7 +10696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="17.25" customHeight="1">
+    <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>184</v>
       </c>
@@ -10271,7 +10712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="17.25" customHeight="1">
+    <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>185</v>
       </c>
@@ -10287,7 +10728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="17.25" customHeight="1">
+    <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>186</v>
       </c>
@@ -10303,7 +10744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="17.25" customHeight="1">
+    <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>187</v>
       </c>
@@ -10319,7 +10760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="17.25" customHeight="1">
+    <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>188</v>
       </c>
@@ -10335,7 +10776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="17.25" customHeight="1">
+    <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>189</v>
       </c>
@@ -10351,7 +10792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="17.25" customHeight="1">
+    <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>190</v>
       </c>
@@ -10367,7 +10808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="17.25" customHeight="1">
+    <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>191</v>
       </c>
@@ -10383,7 +10824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="17.25" customHeight="1">
+    <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>192</v>
       </c>
@@ -10399,7 +10840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="17.25" customHeight="1">
+    <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>193</v>
       </c>
@@ -10415,7 +10856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="17.25" customHeight="1">
+    <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>194</v>
       </c>
@@ -10431,7 +10872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="17.25" customHeight="1">
+    <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>195</v>
       </c>
@@ -10447,7 +10888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="17.25" customHeight="1">
+    <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>196</v>
       </c>
@@ -10463,7 +10904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="17.25" customHeight="1">
+    <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>198</v>
       </c>
@@ -10479,7 +10920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="17.25" customHeight="1">
+    <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>199</v>
       </c>
@@ -10495,7 +10936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="17.25" customHeight="1">
+    <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>200</v>
       </c>
@@ -10511,7 +10952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="17.25" customHeight="1">
+    <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>201</v>
       </c>
@@ -10527,7 +10968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="17.25" customHeight="1">
+    <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>202</v>
       </c>
@@ -10543,7 +10984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="17.25" customHeight="1">
+    <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>203</v>
       </c>
@@ -10559,7 +11000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="17.25" customHeight="1">
+    <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>205</v>
       </c>
@@ -10575,7 +11016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="17.25" customHeight="1">
+    <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>206</v>
       </c>
@@ -10591,20 +11032,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="17.25" customHeight="1">
+    <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>207</v>
       </c>
       <c r="B144" s="19">
         <f ca="1">TODAY()</f>
-        <v>45526</v>
+        <v>45538</v>
       </c>
       <c r="D144" s="2">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="17.25" customHeight="1">
+    <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>208</v>
       </c>
@@ -10620,7 +11061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="17.25" customHeight="1">
+    <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>210</v>
       </c>
@@ -10636,7 +11077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="17.25" customHeight="1">
+    <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>211</v>
       </c>
@@ -10652,7 +11093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="17.25" customHeight="1">
+    <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>213</v>
       </c>
@@ -10668,7 +11109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="17.25" customHeight="1">
+    <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>214</v>
       </c>
@@ -10684,7 +11125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="17.25" customHeight="1">
+    <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>215</v>
       </c>
@@ -10700,7 +11141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="17.25" customHeight="1">
+    <row r="151" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>216</v>
       </c>
@@ -10716,7 +11157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="17.25" customHeight="1">
+    <row r="152" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>217</v>
       </c>
@@ -10732,7 +11173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="17.25" customHeight="1">
+    <row r="153" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>218</v>
       </c>
@@ -10748,7 +11189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="17.25" customHeight="1">
+    <row r="154" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>219</v>
       </c>
@@ -10765,7 +11206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="17.25" customHeight="1">
+    <row r="155" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>220</v>
       </c>
@@ -10781,7 +11222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="17.25" customHeight="1">
+    <row r="156" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>221</v>
       </c>
@@ -10797,7 +11238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="17.25" customHeight="1">
+    <row r="157" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>222</v>
       </c>
@@ -10813,7 +11254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="17.25" customHeight="1">
+    <row r="158" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>223</v>
       </c>
@@ -10829,7 +11270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="17.25" customHeight="1">
+    <row r="159" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>224</v>
       </c>
@@ -10845,7 +11286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="17.25" customHeight="1">
+    <row r="160" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>225</v>
       </c>
@@ -10861,7 +11302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="17.25" customHeight="1">
+    <row r="161" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>226</v>
       </c>
@@ -10877,7 +11318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="17.25" customHeight="1">
+    <row r="162" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>227</v>
       </c>
@@ -10893,7 +11334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="17.25" customHeight="1">
+    <row r="163" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>229</v>
       </c>
@@ -10911,10 +11352,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10934,27 +11375,27 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" outlineLevel="1"/>
-    <col min="11" max="11" width="9.140625" outlineLevel="1" collapsed="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" outlineLevel="1"/>
+    <col min="11" max="11" width="9.109375" outlineLevel="1" collapsed="1"/>
     <col min="12" max="14" width="0" hidden="1" outlineLevel="2"/>
-    <col min="15" max="18" width="9.140625" outlineLevel="1"/>
+    <col min="15" max="18" width="9.109375" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>230</v>
       </c>
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="109" t="s">
+      <c r="D1" s="110" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="109"/>
+      <c r="E1" s="110"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -10962,19 +11403,19 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D3" s="86" t="s">
         <v>235</v>
       </c>
@@ -10982,25 +11423,25 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" customHeight="1">
+    <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:8" outlineLevel="1"/>
-    <row r="11" spans="1:8" outlineLevel="1"/>
-    <row r="12" spans="1:8" hidden="1" outlineLevel="2"/>
-    <row r="13" spans="1:8" hidden="1" outlineLevel="2"/>
-    <row r="14" spans="1:8" hidden="1" outlineLevel="2"/>
-    <row r="15" spans="1:8" outlineLevel="1" collapsed="1"/>
-    <row r="16" spans="1:8" outlineLevel="1"/>
-    <row r="17" outlineLevel="1"/>
-    <row r="18" outlineLevel="1"/>
+    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3"/>
+    <row r="17" outlineLevel="1" x14ac:dyDescent="0.3"/>
+    <row r="18" outlineLevel="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:E2"/>
@@ -11022,14 +11463,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1">
+    <row r="1" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="69" t="s">
         <v>239</v>
       </c>
@@ -11051,7 +11492,7 @@
       </c>
       <c r="M1" s="37"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
         <v>245</v>
       </c>
@@ -11077,7 +11518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
         <v>252</v>
       </c>
@@ -11100,7 +11541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15">
+    <row r="4" spans="1:13" ht="16.2" x14ac:dyDescent="0.4">
       <c r="A4" s="43" t="s">
         <v>256</v>
       </c>
@@ -11126,7 +11567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>262</v>
       </c>
@@ -11146,7 +11587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
         <v>266</v>
       </c>
@@ -11169,7 +11610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
         <v>271</v>
       </c>
@@ -11189,7 +11630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21">
+    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="47" t="s">
         <v>275</v>
       </c>
@@ -11212,7 +11653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="48" t="s">
         <v>280</v>
       </c>
@@ -11229,7 +11670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="49" t="s">
         <v>283</v>
       </c>
@@ -11237,7 +11678,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.5" thickBot="1">
+    <row r="11" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="50" t="s">
         <v>285</v>
       </c>
@@ -11246,7 +11687,7 @@
       </c>
       <c r="F11" s="37"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1">
+    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="51" t="s">
         <v>287</v>
       </c>
@@ -11260,7 +11701,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="52" t="s">
         <v>290</v>
       </c>
@@ -11271,7 +11712,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="53" t="s">
         <v>291</v>
       </c>
@@ -11285,7 +11726,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="54" t="s">
         <v>293</v>
       </c>
@@ -11296,7 +11737,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="55" t="s">
         <v>294</v>
       </c>
@@ -11310,12 +11751,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1">
+    <row r="17" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="56" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" thickBot="1">
+    <row r="18" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="75" t="s">
         <v>297</v>
       </c>
@@ -11327,7 +11768,7 @@
       </c>
       <c r="F18" s="37"/>
     </row>
-    <row r="19" spans="1:6" ht="13.5" thickBot="1">
+    <row r="19" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="76" t="s">
         <v>300</v>
       </c>
@@ -11338,7 +11779,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51.75" thickBot="1">
+    <row r="20" spans="1:6" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="77" t="s">
         <v>303</v>
       </c>
@@ -11352,12 +11793,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5" thickBot="1">
+    <row r="21" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="78" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.5" thickBot="1">
+    <row r="22" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="79" t="s">
         <v>307</v>
       </c>
@@ -11366,13 +11807,13 @@
       </c>
       <c r="E22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="13.5" thickBot="1">
+    <row r="23" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="80" t="s">
         <v>309</v>
       </c>
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+    <row r="24" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="81" t="s">
         <v>310</v>
       </c>
@@ -11381,20 +11822,20 @@
       </c>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
-    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+    <row r="25" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C26" s="68" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
-    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+    <row r="27" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C28" s="89" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.5" thickTop="1"/>
-    <row r="30" spans="1:6">
+    <row r="29" spans="1:6" ht="14.4" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C30" s="88" t="s">
         <v>314</v>
       </c>
@@ -11413,13 +11854,13 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" thickBot="1">
+    <row r="1" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="38" t="s">
         <v>315</v>
       </c>
@@ -11436,7 +11877,7 @@
       <c r="I1" s="37"/>
       <c r="J1" s="37"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>319</v>
       </c>
@@ -11459,7 +11900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
         <v>321</v>
       </c>
@@ -11482,7 +11923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>325</v>
       </c>
@@ -11502,7 +11943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
         <v>328</v>
       </c>
@@ -11526,7 +11967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
         <v>330</v>
       </c>
@@ -11549,7 +11990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
         <v>333</v>
       </c>
@@ -11575,7 +12016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
         <v>337</v>
       </c>
@@ -11586,7 +12027,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="39" t="s">
         <v>339</v>
       </c>
@@ -11595,7 +12036,7 @@
       </c>
       <c r="C9" s="22"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" thickBot="1">
+    <row r="10" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="39" t="s">
         <v>340</v>
       </c>
@@ -11613,7 +12054,7 @@
       <c r="I10" s="37"/>
       <c r="J10" s="37"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="39" t="s">
         <v>342</v>
       </c>
@@ -11636,13 +12077,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="39" t="s">
         <v>344</v>
       </c>
       <c r="B12" s="40">
         <f ca="1">TODAY()</f>
-        <v>45526</v>
+        <v>45538</v>
       </c>
       <c r="C12" s="40">
         <f>DATE(2010,10,2)</f>
@@ -11661,7 +12102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="39" t="s">
         <v>346</v>
       </c>
@@ -11684,7 +12125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="39" t="s">
         <v>348</v>
       </c>
@@ -11710,7 +12151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="39" t="s">
         <v>350</v>
       </c>
@@ -11730,7 +12171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="39" t="s">
         <v>352</v>
       </c>
@@ -11753,7 +12194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="39" t="s">
         <v>354</v>
       </c>
@@ -11776,7 +12217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="39" t="s">
         <v>356</v>
       </c>
@@ -11799,7 +12240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="39" t="s">
         <v>358</v>
       </c>
@@ -11822,7 +12263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="39" t="s">
         <v>360</v>
       </c>
@@ -11845,7 +12286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="39" t="s">
         <v>362</v>
       </c>
@@ -11871,7 +12312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="39" t="s">
         <v>364</v>
       </c>
@@ -11897,7 +12338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>366</v>
       </c>
@@ -11923,7 +12364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G24" s="35" t="s">
         <v>368</v>
       </c>
@@ -11940,7 +12381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
         <v>369</v>
       </c>
@@ -11966,7 +12407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G26" s="35" t="s">
         <v>371</v>
       </c>
@@ -11986,7 +12427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>372</v>
       </c>
@@ -12012,7 +12453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G28" s="35" t="s">
         <v>374</v>
       </c>
@@ -12032,7 +12473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G29" s="35" t="s">
         <v>375</v>
       </c>
@@ -12052,7 +12493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G30" s="35" t="s">
         <v>376</v>
       </c>
@@ -12072,7 +12513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.5" thickBot="1">
+    <row r="31" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G31" s="36" t="s">
         <v>377</v>
       </c>
@@ -12086,7 +12527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G32" s="35" t="s">
         <v>378</v>
       </c>
@@ -12100,7 +12541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="7:10">
+    <row r="33" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G33" s="35" t="s">
         <v>379</v>
       </c>
@@ -12114,7 +12555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:10">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G34" s="35" t="s">
         <v>380</v>
       </c>
@@ -12128,7 +12569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="7:10">
+    <row r="35" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G35" s="35" t="s">
         <v>381</v>
       </c>
@@ -12142,7 +12583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:10">
+    <row r="36" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G36" s="35" t="s">
         <v>382</v>
       </c>
@@ -12156,7 +12597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:10">
+    <row r="37" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G37" s="35" t="s">
         <v>383</v>
       </c>
@@ -12170,110 +12611,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:10">
+    <row r="39" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G39" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="40" priority="58">
+    <cfRule type="expression" dxfId="22" priority="58">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="39" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="38" priority="114"/>
+    <cfRule type="aboveAverage" dxfId="20" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="37" priority="73" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="19" priority="73" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="36" priority="71">
+    <cfRule type="containsBlanks" dxfId="18" priority="71">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="35" priority="70">
+    <cfRule type="containsErrors" dxfId="17" priority="70">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="34" priority="69" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="16" priority="69" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="33" priority="67" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="15" priority="67" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="66">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="31" priority="65">
+    <cfRule type="notContainsErrors" dxfId="13" priority="65">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="30" priority="64" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="12" priority="64" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="29" priority="63" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="11" priority="63" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="28" priority="115" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="115" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="27" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="45" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="26" priority="56" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="56" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
@@ -12307,10 +12748,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="19" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="18" priority="96"/>
+    <cfRule type="uniqueValues" dxfId="0" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="44">
@@ -12738,24 +13179,24 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C3" s="18" t="s">
         <v>35</v>
       </c>
@@ -12781,7 +13222,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>42</v>
       </c>
@@ -12812,7 +13253,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>44</v>
       </c>
@@ -12843,7 +13284,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>391</v>
       </c>
@@ -12876,7 +13317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>392</v>
       </c>
@@ -12887,7 +13328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>3</v>
       </c>
@@ -12895,7 +13336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>393</v>
       </c>
@@ -12906,7 +13347,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>3</v>
       </c>
@@ -12914,7 +13355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>396</v>
       </c>
@@ -12925,7 +13366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>3</v>
       </c>
@@ -12933,7 +13374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>397</v>
       </c>
@@ -12944,7 +13385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>3</v>
       </c>
@@ -12952,7 +13393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>398</v>
       </c>
@@ -12963,7 +13404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>3</v>
       </c>
@@ -12971,7 +13412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>399</v>
       </c>
@@ -12982,7 +13423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>3</v>
       </c>
@@ -12990,7 +13431,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>400</v>
       </c>
@@ -13001,7 +13442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>3</v>
       </c>
@@ -13009,7 +13450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>391</v>
       </c>
@@ -13018,7 +13459,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>401</v>
       </c>
@@ -13029,7 +13470,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="31" spans="2:4" hidden="1">
+    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>404</v>
       </c>
@@ -13037,7 +13478,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>405</v>
       </c>
@@ -13045,7 +13486,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>406</v>
       </c>
@@ -13075,28 +13516,28 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="93" t="s">
         <v>407</v>
       </c>
@@ -13106,7 +13547,7 @@
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -13114,7 +13555,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="90" t="s">
@@ -13124,7 +13565,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="90" t="s">
@@ -13158,7 +13599,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="91" t="s">
@@ -13171,7 +13612,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="92">
@@ -13184,7 +13625,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="91" t="s">
@@ -13197,7 +13638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="92">
@@ -13210,7 +13651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="91" t="s">
@@ -13223,7 +13664,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="92">
@@ -13236,7 +13677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="91" t="s">
         <v>44</v>
       </c>
@@ -13247,7 +13688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="92">
         <v>23000</v>
       </c>
@@ -13258,7 +13699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="91" t="s">
         <v>50</v>
       </c>
@@ -13269,7 +13710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="92">
         <v>2</v>
       </c>
@@ -13280,7 +13721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="91" t="s">
         <v>48</v>
       </c>
@@ -13291,7 +13732,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="92">
         <v>50024</v>
       </c>
@@ -13302,7 +13743,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="3:12">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="91" t="s">
         <v>53</v>
       </c>
@@ -13313,7 +13754,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="3:12">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="92">
         <v>189576</v>
       </c>
@@ -13324,7 +13765,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:12">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="91" t="s">
         <v>57</v>
       </c>
@@ -13335,7 +13776,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="3:12">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="92">
         <v>5000</v>
       </c>
@@ -13346,7 +13787,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:12">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="91" t="s">
         <v>411</v>
       </c>
@@ -13388,33 +13829,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="B49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="26" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="65.109375" customWidth="1"/>
+    <col min="2" max="26" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>413</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>415</v>
       </c>
@@ -13433,9 +13874,9 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="38.25">
+    <row r="1" spans="1:1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A1" s="100" t="s">
         <v>416</v>
       </c>

</xml_diff>

<commit_message>
[IMP] sheet: add sheet color
This commits adds the possibility to color the sheet tab in the
bottom bar.

closes odoo/o-spreadsheet#4888

Task: 4088710
Signed-off-by: Rémi Rahir (rar) <rar@odoo.com>
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82EC8D04-FB30-4625-805F-DD659B4B146F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{05E556DF-B6A9-4914-8E28-82201545992C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
   </externalReferences>
   <calcPr calcId="191028" calcCompleted="0"/>
   <pivotCaches>
-    <pivotCache cacheId="828" r:id="rId15"/>
+    <pivotCache cacheId="153" r:id="rId15"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2240,7 +2240,7 @@
         <u/>
         <color theme="7"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="171" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="lightTrellis">
           <fgColor theme="4"/>
@@ -2795,6 +2795,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FF000000"/>
       <color rgb="FFCECECE"/>
       <color rgb="FFD0CECE"/>
@@ -6942,7 +6943,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="828" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="153" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -7525,9 +7526,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385D5EBC-45F5-4C42-AA75-560DF70B9F2E}">
+  <sheetPr>
+    <tabColor rgb="FF00FF00"/>
+  </sheetPr>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -8041,6 +8045,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0630FA18-71FC-4ACD-8379-39A3603D1DD6}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
   <dimension ref="A1:R163"/>
   <sheetViews>
     <sheetView topLeftCell="A97" workbookViewId="0">
@@ -9900,7 +9907,7 @@
       </c>
       <c r="B100" s="20">
         <f ca="1">NOW()</f>
-        <v>45512.434189004627</v>
+        <v>45526.511599421297</v>
       </c>
       <c r="D100" s="2">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
@@ -10590,7 +10597,7 @@
       </c>
       <c r="B144" s="19">
         <f ca="1">TODAY()</f>
-        <v>45512</v>
+        <v>45526</v>
       </c>
       <c r="D144" s="2">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
@@ -10918,12 +10925,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FE33AE-060F-4630-8DDE-76E5F5CF58F5}">
   <sheetPr>
+    <tabColor rgb="FFFF0000"/>
     <outlinePr summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -11634,7 +11642,7 @@
       </c>
       <c r="B12" s="40">
         <f ca="1">TODAY()</f>
-        <v>45512</v>
+        <v>45526</v>
       </c>
       <c r="C12" s="40">
         <f>DATE(2010,10,2)</f>
@@ -13380,7 +13388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>

</xml_diff>